<commit_message>
Finalisacao dos precessos para gerar os dandos completos
</commit_message>
<xml_diff>
--- a/Dados processados.xlsx
+++ b/Dados processados.xlsx
@@ -573,7 +573,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -611,6 +611,16 @@
       </c>
       <c r="B3" t="n">
         <v>6915</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>perc_sim</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>49.83</v>
       </c>
     </row>
   </sheetData>
@@ -758,7 +768,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SPLIT 18001 À 30000</t>
+          <t>SPLIT 10001 À 18000</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -768,7 +778,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SPLIT 10001 À 18000</t>
+          <t>SPLIT 18001 À 30000</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -778,7 +788,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>JANELA 8501 À 10000</t>
+          <t>JANELA ATÉ 8500 BTUS</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -788,7 +798,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>KIT COZINHA DE AÇO</t>
+          <t>TV LED DE 48" À 54"</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -798,7 +808,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SYSTEM</t>
+          <t>GRILL</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -808,7 +818,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>GRILL</t>
+          <t>SANDUICHEIRA</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -818,7 +828,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>TV 4K DE 60" À 69"</t>
+          <t>SMART MULTISIM LIVRE</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -828,7 +838,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>JANELA ATÉ 8500 BTUS</t>
+          <t>CAFETEIRA</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -838,7 +848,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>SANDUICHEIRA</t>
+          <t>TV 4K DE 60" À 69"</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -848,7 +858,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>FERRO SECO</t>
+          <t>TV 4K ATÉ 59"</t>
         </is>
       </c>
       <c r="B11" t="n">

</xml_diff>